<commit_message>
v0.5.0 is convRates defines as a parameter instead of in-model calculus
also first sim script for SA ready (hardest one,  the others will just be modification of this one)
</commit_message>
<xml_diff>
--- a/SAparameterTable.xlsx
+++ b/SAparameterTable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Parameter</t>
   </si>
@@ -39,12 +39,6 @@
     <t>OFAT</t>
   </si>
   <si>
-    <t>Generalist</t>
-  </si>
-  <si>
-    <t>Rank prey types at random</t>
-  </si>
-  <si>
     <t>{0;1}</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Rank prey types by preference</t>
   </si>
   <si>
-    <t>Predator regime</t>
-  </si>
-  <si>
     <t>Predator efficiency</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>Prey catch probability ratio</t>
   </si>
   <si>
-    <t>Predation assymetry</t>
-  </si>
-  <si>
     <t>Firness advantage of a prey over the other</t>
   </si>
   <si>
@@ -124,6 +112,12 @@
   </si>
   <si>
     <t>Potential AC-inducing factors</t>
+  </si>
+  <si>
+    <t>Predation asymmetry</t>
+  </si>
+  <si>
+    <t>Regime</t>
   </si>
 </sst>
 </file>
@@ -162,18 +156,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -261,51 +249,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -651,31 +633,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="2" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="45">
-      <c r="A2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="13"/>
+      <c r="A2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,8 +667,8 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
@@ -695,274 +677,253 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="1:8" ht="60">
+      <c r="A3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1</v>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45">
-      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90">
+      <c r="A11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="60">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="45">
+      <c r="A12" s="10"/>
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="90">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="75">
+      <c r="A13" s="10"/>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="75">
+      <c r="A14" s="10"/>
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="90">
-      <c r="A12" s="4" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="75">
+      <c r="A15" s="10"/>
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="45">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="75">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="75">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="75">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>